<commit_message>
Added more tests and PET module and helper methods
</commit_message>
<xml_diff>
--- a/testData/UserData.xlsx
+++ b/testData/UserData.xlsx
@@ -34,7 +34,7 @@
     <t>phone</t>
   </si>
   <si>
-    <t>aiymaUser1</t>
+    <t>testUser55445201</t>
   </si>
   <si>
     <t>John</t>
@@ -49,7 +49,7 @@
     <t>test@1</t>
   </si>
   <si>
-    <t>aiymaUser2</t>
+    <t>testUser55445202</t>
   </si>
   <si>
     <t>Kim</t>
@@ -64,7 +64,7 @@
     <t>test@2</t>
   </si>
   <si>
-    <t>aiymaUser3</t>
+    <t>testUser55445203</t>
   </si>
   <si>
     <t>Smith</t>
@@ -407,7 +407,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>1111.0</v>
+        <v>5.5445201E7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3">
-        <v>2222.0</v>
+        <v>5.5445202E7</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3">
-        <v>3333.0</v>
+        <v>5.5445203E7</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>

</xml_diff>